<commit_message>
fix(tui): calculate correct hours
</commit_message>
<xml_diff>
--- a/runtime/asistencia/asistencia.xlsx
+++ b/runtime/asistencia/asistencia.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,7 +494,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>presente</t>
+          <t>ausente</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -639,6 +639,29 @@
         <v>11</v>
       </c>
       <c r="E9" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1234</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>fdsafdasfs</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>ausente</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>9</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>B</t>
         </is>

</xml_diff>